<commit_message>
added batch file to launch app
</commit_message>
<xml_diff>
--- a/files/Templates/collected_data.xlsx
+++ b/files/Templates/collected_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marpo\Documents\Research\STICS\Code\mkSTICSfiles\files\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{17F29D40-148B-466A-98D2-AD40EA1FE053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B2079A-76F3-4845-AD5F-CC3D716C6DB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="soils" sheetId="5" r:id="rId2"/>
     <sheet name="stations" sheetId="6" r:id="rId3"/>
     <sheet name="usms" sheetId="1" r:id="rId4"/>
-    <sheet name="info" sheetId="4" r:id="rId5"/>
+    <sheet name="options" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="Fertilizer_Application">Table3[Fertilizer_Application]</definedName>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="151">
   <si>
     <t>usm_name</t>
   </si>
@@ -427,13 +427,88 @@
   </si>
   <si>
     <t>k</t>
+  </si>
+  <si>
+    <t>SOM_1</t>
+  </si>
+  <si>
+    <t>SON_1</t>
+  </si>
+  <si>
+    <t>CN_ratio</t>
+  </si>
+  <si>
+    <t>FC_1_unit</t>
+  </si>
+  <si>
+    <t>WP_1_unit</t>
+  </si>
+  <si>
+    <t>FC_2_unit</t>
+  </si>
+  <si>
+    <t>WP_2_unit</t>
+  </si>
+  <si>
+    <t>FC_3_unit</t>
+  </si>
+  <si>
+    <t>WP_3_unit</t>
+  </si>
+  <si>
+    <t>FC_4_unit</t>
+  </si>
+  <si>
+    <t>WP_4_unit</t>
+  </si>
+  <si>
+    <t>Soil Moisture Units</t>
+  </si>
+  <si>
+    <t>% g/g</t>
+  </si>
+  <si>
+    <t>% V/V</t>
+  </si>
+  <si>
+    <t>initial_NO3_1_units</t>
+  </si>
+  <si>
+    <t>initial_NH4_1_units</t>
+  </si>
+  <si>
+    <t>initial_NO3_2_unit</t>
+  </si>
+  <si>
+    <t>initial_NH4_2_unit</t>
+  </si>
+  <si>
+    <t>initial_NO3_3_unit</t>
+  </si>
+  <si>
+    <t>initial_NH4_3_unit</t>
+  </si>
+  <si>
+    <t>initial_NO3_4_unit</t>
+  </si>
+  <si>
+    <t>initial_NH4_4_unit</t>
+  </si>
+  <si>
+    <t>kg N/ha.</t>
+  </si>
+  <si>
+    <t>mg N/ha.</t>
+  </si>
+  <si>
+    <t>Nitrogen Units</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,13 +523,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -554,6 +646,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF7C80"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFEF2EC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFBEF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEFF6EA"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFECF4FA"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -676,9 +792,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -693,31 +809,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -726,40 +835,105 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="35">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -785,6 +959,50 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="hair">
@@ -834,157 +1052,16 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <right style="thin">
           <color indexed="64"/>
         </right>
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border outline="0">
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="hair">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
       </border>
     </dxf>
     <dxf>
@@ -1039,9 +1116,88 @@
     </dxf>
     <dxf>
       <border outline="0">
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
         <bottom style="medium">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="hair">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -1051,10 +1207,31 @@
         </right>
       </border>
     </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFECF4FA"/>
+      <color rgb="FFEFF6EA"/>
+      <color rgb="FFFFFBEF"/>
+      <color rgb="FFFFF5D9"/>
+      <color rgb="FFFEF2EC"/>
       <color rgb="FFFF7C80"/>
       <color rgb="FFFFCCCC"/>
     </mruColors>
@@ -1071,24 +1248,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1AD7F1BC-9C4F-46C6-88D5-D2D5C340F1D9}" name="Table6" displayName="Table6" ref="A2:AT3" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="6" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{1AD7F1BC-9C4F-46C6-88D5-D2D5C340F1D9}" name="Table6" displayName="Table6" ref="A2:AT3" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32">
   <autoFilter ref="A2:AT3" xr:uid="{1AD7F1BC-9C4F-46C6-88D5-D2D5C340F1D9}"/>
   <tableColumns count="46">
-    <tableColumn id="1" xr3:uid="{6B129591-A0EC-4CC8-AA8E-70259B5C9131}" name="file_name" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{1FBFF361-0229-404E-A60E-FCEC995B36AD}" name="year" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{6B129591-A0EC-4CC8-AA8E-70259B5C9131}" name="file_name" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{1FBFF361-0229-404E-A60E-FCEC995B36AD}" name="year" dataDxfId="30"/>
     <tableColumn id="3" xr3:uid="{416116E5-319A-4096-B7E5-AF8ADEF0E80A}" name="tillage_date"/>
-    <tableColumn id="4" xr3:uid="{781FB9F7-258C-4E50-8A90-CAA110FA989E}" name="tillage_depth" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{781FB9F7-258C-4E50-8A90-CAA110FA989E}" name="tillage_depth" dataDxfId="29"/>
     <tableColumn id="5" xr3:uid="{A768ED69-1CCB-4A41-99C1-D5042177408B}" name="planting_date"/>
     <tableColumn id="6" xr3:uid="{5517C570-4D1C-46EC-9FB0-4FEA929440E1}" name="planting_depth"/>
-    <tableColumn id="7" xr3:uid="{8F3D9EFB-6197-44D6-9CAB-532096E5D0DE}" name="plants_per_m2" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{8F3D9EFB-6197-44D6-9CAB-532096E5D0DE}" name="plants_per_m2" dataDxfId="28"/>
     <tableColumn id="8" xr3:uid="{7DEB259C-DAE3-4A1E-B476-951FEF30ABD2}" name="emergence"/>
     <tableColumn id="9" xr3:uid="{8590CC43-CF1F-45A9-A612-CE3749B53C84}" name="flowering"/>
-    <tableColumn id="10" xr3:uid="{DAF1F67C-7CB4-4AD2-B1D4-24884C7C9D57}" name="maturity" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{DAF1F67C-7CB4-4AD2-B1D4-24884C7C9D57}" name="maturity" dataDxfId="27"/>
     <tableColumn id="11" xr3:uid="{1651DE3B-149A-4121-AFB0-BA33E8308050}" name="application_date"/>
     <tableColumn id="12" xr3:uid="{358B23A5-F859-4B79-9182-F98F3D69F461}" name="kg_N_per_ha"/>
     <tableColumn id="13" xr3:uid="{FEB67719-45D9-4389-A438-548C552EBED6}" name="fert_type"/>
     <tableColumn id="14" xr3:uid="{B9B3005C-6E63-4AA3-BE8E-646D9659B76F}" name="fert_location"/>
-    <tableColumn id="15" xr3:uid="{F5737449-F543-4637-B8F3-6DBD1B98EDA2}" name="fert_depth" dataDxfId="0"/>
+    <tableColumn id="15" xr3:uid="{F5737449-F543-4637-B8F3-6DBD1B98EDA2}" name="fert_depth" dataDxfId="26"/>
     <tableColumn id="16" xr3:uid="{AA12C7D8-D645-4337-B05C-CB5F5C197AE4}" name="irrigation_date_1"/>
     <tableColumn id="17" xr3:uid="{017BC113-D478-4E04-AEE6-020CA6B48738}" name="amount_1"/>
     <tableColumn id="18" xr3:uid="{498ED556-89DC-49A5-A6C1-DF741DBED2EF}" name="irrigation_date_2"/>
@@ -1126,77 +1303,96 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{34F446AA-1543-42D0-AA83-3EA91742E62F}" name="Table7" displayName="Table7" ref="A2:AL3" totalsRowShown="0" headerRowDxfId="15" headerRowBorderDxfId="20" tableBorderDxfId="21">
-  <autoFilter ref="A2:AL3" xr:uid="{34F446AA-1543-42D0-AA83-3EA91742E62F}"/>
-  <tableColumns count="38">
-    <tableColumn id="1" xr3:uid="{4674EE1C-2CD4-485E-8B27-A14DEFFAAD8A}" name="soil_profile_name" dataDxfId="19"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{34F446AA-1543-42D0-AA83-3EA91742E62F}" name="Table7" displayName="Table7" ref="A2:BE3" totalsRowShown="0" headerRowDxfId="13" headerRowBorderDxfId="11" tableBorderDxfId="12">
+  <autoFilter ref="A2:BE3" xr:uid="{34F446AA-1543-42D0-AA83-3EA91742E62F}"/>
+  <tableColumns count="57">
+    <tableColumn id="1" xr3:uid="{4674EE1C-2CD4-485E-8B27-A14DEFFAAD8A}" name="soil_profile_name" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{72D785FE-A1AF-4E08-AB14-39FAD15DB9BD}" name="thickness_1"/>
     <tableColumn id="3" xr3:uid="{1838D7E8-2B3C-471C-9A0B-D70D91F18417}" name="pH"/>
     <tableColumn id="4" xr3:uid="{22C3A2D3-19B8-4556-9BAC-DEDF286C1C2C}" name="%_sand_1"/>
     <tableColumn id="5" xr3:uid="{1040C5A7-CB33-4419-8EA9-5541F66164AB}" name="%_clay_1"/>
     <tableColumn id="6" xr3:uid="{B2FB90E9-0C4B-4F1F-8CF8-A6B1B8736BCF}" name="BD_1"/>
+    <tableColumn id="39" xr3:uid="{E2BB7CB7-ACCE-4FF1-AF91-42C43097A8A0}" name="SOM_1"/>
     <tableColumn id="7" xr3:uid="{20FE986C-6B28-4993-A555-F2428095534E}" name="SOC_1"/>
+    <tableColumn id="40" xr3:uid="{EC836542-6DD7-49C9-82D9-B724BCE18341}" name="SON_1"/>
+    <tableColumn id="41" xr3:uid="{F7750E58-5B0E-4494-87AF-B025671824DE}" name="CN_ratio"/>
     <tableColumn id="8" xr3:uid="{0592115C-328E-42C4-B9CB-D43026D4FC27}" name="FC_1"/>
+    <tableColumn id="42" xr3:uid="{5C21A417-1737-43F1-BC15-EC087A009A68}" name="FC_1_unit"/>
     <tableColumn id="9" xr3:uid="{C1383A59-387E-4667-852A-B0CF467088F3}" name="WP_1"/>
+    <tableColumn id="43" xr3:uid="{75E60C07-9873-41B6-AB5A-253087B95CFA}" name="WP_1_unit"/>
     <tableColumn id="10" xr3:uid="{34D0D911-5DB4-457F-88A7-76A42B57EE1A}" name="initial_NO3_1"/>
-    <tableColumn id="11" xr3:uid="{58B6280A-10C4-4120-9FF8-93150CE70C6B}" name="initial_NH4_1" dataDxfId="18"/>
+    <tableColumn id="52" xr3:uid="{630D852C-736F-4D0D-8BB3-6EB32B59A383}" name="initial_NO3_1_units"/>
+    <tableColumn id="53" xr3:uid="{CEF78893-60AA-4A20-A771-E76562B8EBC1}" name="initial_NH4_1"/>
+    <tableColumn id="11" xr3:uid="{58B6280A-10C4-4120-9FF8-93150CE70C6B}" name="initial_NH4_1_units" dataDxfId="9"/>
     <tableColumn id="12" xr3:uid="{FD043EB5-2678-4920-8D76-EBE8316E27AA}" name="thickness_2"/>
     <tableColumn id="13" xr3:uid="{F124AE04-B447-4F21-A0E8-7B26199C0F49}" name="%_sand_2"/>
     <tableColumn id="14" xr3:uid="{F119498A-3A35-40E3-A753-7CF13D724118}" name="%_clay_2"/>
     <tableColumn id="15" xr3:uid="{AE51522F-6903-42D4-88CE-A95BCE8C77EF}" name="BD_2"/>
     <tableColumn id="16" xr3:uid="{12076489-6AD7-4297-A729-20EF93AEE58D}" name="SOC_2"/>
     <tableColumn id="17" xr3:uid="{D6D5EFD4-69CC-4AF2-8C6B-0B430468C4C2}" name="FC_2"/>
+    <tableColumn id="44" xr3:uid="{7158FD96-C69C-40D1-A3B8-2D043DF66D42}" name="FC_2_unit"/>
     <tableColumn id="18" xr3:uid="{BBF6A61D-2092-4DF7-8C38-9024164291AE}" name="WP_2"/>
+    <tableColumn id="45" xr3:uid="{2A662E87-2699-41FA-AF9F-C807E1C2112B}" name="WP_2_unit"/>
     <tableColumn id="19" xr3:uid="{BB4B796C-CA3E-424C-87B0-4BF33581B61B}" name="initial_NO3_2"/>
-    <tableColumn id="20" xr3:uid="{613F6ECB-AFEC-4E8A-BD78-2579E90B1783}" name="initial_NH4_2" dataDxfId="17"/>
+    <tableColumn id="54" xr3:uid="{13CDB225-A28A-424D-943F-330A6ABE0CF2}" name="initial_NO3_2_unit"/>
+    <tableColumn id="55" xr3:uid="{333E59C3-3A13-4C92-9169-AC90D5E5D3EB}" name="initial_NH4_2"/>
+    <tableColumn id="20" xr3:uid="{613F6ECB-AFEC-4E8A-BD78-2579E90B1783}" name="initial_NH4_2_unit" dataDxfId="8"/>
     <tableColumn id="21" xr3:uid="{5D7B3549-7F90-410E-90FF-149F4376EBB7}" name="thickness_3"/>
     <tableColumn id="22" xr3:uid="{6C917DE4-8D95-496E-A6F1-EAB7450774EE}" name="%_sand_3"/>
     <tableColumn id="23" xr3:uid="{90DE7FE2-3A23-4294-8BD0-2D321FF71179}" name="%_clay_3"/>
     <tableColumn id="24" xr3:uid="{C874CBBB-CB06-4239-AE9B-72564A3EDC14}" name="BD_3"/>
     <tableColumn id="25" xr3:uid="{49CED3FB-E83C-4973-A99D-DAC6B3AFC7B1}" name="SOC_3"/>
     <tableColumn id="26" xr3:uid="{63FB3901-EBED-4379-9E9C-83064A8ADD01}" name="FC_3"/>
+    <tableColumn id="47" xr3:uid="{5C201AAC-779E-4362-9603-51762D2AD5CF}" name="FC_3_unit"/>
     <tableColumn id="27" xr3:uid="{6EEACF0E-3934-49DF-9991-42C2DB718BE0}" name="WP_3"/>
+    <tableColumn id="48" xr3:uid="{67EEF171-24DC-4B50-B1F4-746B04E8F368}" name="WP_3_unit"/>
     <tableColumn id="28" xr3:uid="{7AAE3F1E-C60E-4E11-A023-F09548D5AA39}" name="initial_NO3_3"/>
-    <tableColumn id="29" xr3:uid="{4BF74EC8-B9F2-42F0-AA7F-7CF70391A1FD}" name="initial_NH4_3" dataDxfId="16"/>
+    <tableColumn id="56" xr3:uid="{2B23B0A6-3617-432B-8EEA-E2AC0892F317}" name="initial_NO3_3_unit"/>
+    <tableColumn id="57" xr3:uid="{1D0A3587-38DB-4073-B5D4-36DA82425955}" name="initial_NH4_3"/>
+    <tableColumn id="29" xr3:uid="{4BF74EC8-B9F2-42F0-AA7F-7CF70391A1FD}" name="initial_NH4_3_unit" dataDxfId="7"/>
     <tableColumn id="30" xr3:uid="{4F55D6E9-95FD-4FC3-8012-EBB0DDAD9C3D}" name="thickness_4"/>
     <tableColumn id="31" xr3:uid="{4C1178FA-055B-4F19-A181-638D37A24EB6}" name="%_sand_4"/>
     <tableColumn id="32" xr3:uid="{7BBFA3FD-BBE5-4B68-A551-EFDEA7062540}" name="%_clay_4"/>
     <tableColumn id="33" xr3:uid="{D0607A27-FB9E-4DA9-A7F3-7A932B2608A4}" name="BD_4"/>
     <tableColumn id="34" xr3:uid="{BD46131F-AB56-411A-8742-B77FBBE1967B}" name="SOC_4"/>
     <tableColumn id="35" xr3:uid="{EC2EEDB8-3CC6-4DEE-9309-DBA3B11A2D16}" name="FC_4"/>
-    <tableColumn id="36" xr3:uid="{2FE3E094-F831-4B6A-8F68-958367A1890E}" name="WP_4"/>
-    <tableColumn id="37" xr3:uid="{8064862C-F8DC-4543-B5CF-D282DD564B1D}" name="initial_NO3_4"/>
-    <tableColumn id="38" xr3:uid="{251884D5-BA16-4F6E-89D1-06011C0ABD02}" name="initial_NH4_4"/>
+    <tableColumn id="50" xr3:uid="{D1D16E63-48A7-4CF1-950A-55FD748CC035}" name="FC_4_unit" dataDxfId="6"/>
+    <tableColumn id="36" xr3:uid="{2FE3E094-F831-4B6A-8F68-958367A1890E}" name="WP_4" dataDxfId="5"/>
+    <tableColumn id="51" xr3:uid="{FDA92DA7-3473-43EC-9CF7-2973FA9CC4D4}" name="WP_4_unit" dataDxfId="4"/>
+    <tableColumn id="58" xr3:uid="{BE460051-3822-4F7B-9128-B9FF3E679D50}" name="initial_NO3_4" dataDxfId="3"/>
+    <tableColumn id="37" xr3:uid="{8064862C-F8DC-4543-B5CF-D282DD564B1D}" name="initial_NO3_4_unit" dataDxfId="2"/>
+    <tableColumn id="59" xr3:uid="{17C5A0C3-B5F4-4AAB-876C-FC876098B9C8}" name="initial_NH4_4" dataDxfId="1"/>
+    <tableColumn id="38" xr3:uid="{251884D5-BA16-4F6E-89D1-06011C0ABD02}" name="initial_NH4_4_unit" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{16C387FE-1D31-45D4-9107-29718893990C}" name="Table5" displayName="Table5" ref="A1:D2" totalsRowShown="0" headerRowBorderDxfId="26" tableBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{16C387FE-1D31-45D4-9107-29718893990C}" name="Table5" displayName="Table5" ref="A1:D2" totalsRowShown="0" headerRowBorderDxfId="25" tableBorderDxfId="24">
   <autoFilter ref="A1:D2" xr:uid="{16C387FE-1D31-45D4-9107-29718893990C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9BCD565A-9AEA-41E2-A4E9-5770EC475FD6}" name="station_name" dataDxfId="25"/>
-    <tableColumn id="2" xr3:uid="{2FFE488A-7A94-4C6D-BFBF-9D19F7354A7D}" name="latitude" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{7A348C5F-5ECA-4DC4-9498-87CB7828B623}" name="PET_calculation" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{528CFAC7-D6A1-4BF3-A218-92AEE6E73C93}" name="average_windspeed" dataDxfId="22"/>
+    <tableColumn id="1" xr3:uid="{9BCD565A-9AEA-41E2-A4E9-5770EC475FD6}" name="station_name" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{2FFE488A-7A94-4C6D-BFBF-9D19F7354A7D}" name="latitude" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{7A348C5F-5ECA-4DC4-9498-87CB7828B623}" name="PET_calculation" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{528CFAC7-D6A1-4BF3-A218-92AEE6E73C93}" name="average_windspeed" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{0F5B8E89-2F05-4CC0-ACA9-79A38A5A9857}" name="Table8" displayName="Table8" ref="A2:J3" totalsRowShown="0" headerRowBorderDxfId="13" tableBorderDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{0F5B8E89-2F05-4CC0-ACA9-79A38A5A9857}" name="Table8" displayName="Table8" ref="A2:J3" totalsRowShown="0" headerRowBorderDxfId="19" tableBorderDxfId="18">
   <autoFilter ref="A2:J3" xr:uid="{0F5B8E89-2F05-4CC0-ACA9-79A38A5A9857}"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{524AE2E3-B113-41B0-849D-8331462FB910}" name="usm_name" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{524AE2E3-B113-41B0-849D-8331462FB910}" name="usm_name" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{C58B90D4-B75A-409B-9D58-E09932ABF65C}" name="simulation_start"/>
-    <tableColumn id="3" xr3:uid="{DDB99A97-7CAB-4C4A-87B0-F44791A69661}" name="simulation_end" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{DDB99A97-7CAB-4C4A-87B0-F44791A69661}" name="simulation_end" dataDxfId="16"/>
     <tableColumn id="4" xr3:uid="{CA3AF775-2448-4D7D-9193-B5BBEE39AD09}" name="management_file_name"/>
     <tableColumn id="5" xr3:uid="{C4CB74A7-2660-4D67-9D08-D7802D112D6D}" name="soil_profile_name"/>
     <tableColumn id="6" xr3:uid="{EE8564A9-D685-42B6-914D-B5F77F840B11}" name="weather_station_name"/>
-    <tableColumn id="7" xr3:uid="{DF70C6E4-2795-4D3D-B86B-8B48BE8FB3E1}" name="plant_file" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{B3D6750F-E334-4A3F-A048-BA40F1D2EC0C}" name="cultivar_code" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{DF70C6E4-2795-4D3D-B86B-8B48BE8FB3E1}" name="plant_file" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{B3D6750F-E334-4A3F-A048-BA40F1D2EC0C}" name="cultivar_code" dataDxfId="14"/>
     <tableColumn id="9" xr3:uid="{BDB57316-D9C6-4EE3-821F-F5561E0078D9}" name="first_year"/>
     <tableColumn id="10" xr3:uid="{733885B2-6768-4BD5-9F65-4E7F4F6262F5}" name="last_year"/>
   </tableColumns>
@@ -1229,6 +1425,26 @@
   <autoFilter ref="E1:E3" xr:uid="{6A574AAF-4FAA-4157-AC4A-8B9D21C891D1}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{36475FCB-C73B-4857-BA9C-894911E4A8A7}" name="Fertilizer_Application"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8070D148-86D5-42F4-953C-3FD3B59B038F}" name="Table4" displayName="Table4" ref="G1:G3" totalsRowShown="0">
+  <autoFilter ref="G1:G3" xr:uid="{8070D148-86D5-42F4-953C-3FD3B59B038F}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{8C51BBDC-E41E-4966-B7A2-2ADDB3FCD779}" name="Soil Moisture Units"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{38082219-60DA-4A2D-BE84-54584CE20A1B}" name="Table9" displayName="Table9" ref="I1:I3" totalsRowShown="0">
+  <autoFilter ref="I1:I3" xr:uid="{38082219-60DA-4A2D-BE84-54584CE20A1B}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{79460CD6-4F26-4C6D-8875-F9DB638BEE07}" name="Nitrogen Units"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1497,6 +1713,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC9ADCD5-143F-4315-B1FA-DA42E99C8884}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:AT3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -1557,198 +1776,198 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="19" t="s">
+      <c r="D1" s="26"/>
+      <c r="E1" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="24" t="s">
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="23" t="s">
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="22" t="s">
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-      <c r="S1" s="22"/>
-      <c r="T1" s="22"/>
-      <c r="U1" s="22"/>
-      <c r="V1" s="22"/>
-      <c r="W1" s="22"/>
-      <c r="X1" s="22"/>
-      <c r="Y1" s="22"/>
-      <c r="Z1" s="22"/>
-      <c r="AA1" s="22"/>
-      <c r="AB1" s="22"/>
-      <c r="AC1" s="22"/>
-      <c r="AD1" s="22"/>
-      <c r="AE1" s="22"/>
-      <c r="AF1" s="22"/>
-      <c r="AG1" s="22"/>
-      <c r="AH1" s="22"/>
-      <c r="AI1" s="22"/>
-      <c r="AJ1" s="22"/>
-      <c r="AK1" s="22"/>
-      <c r="AL1" s="22"/>
-      <c r="AM1" s="22"/>
-      <c r="AN1" s="22"/>
-      <c r="AO1" s="22"/>
-      <c r="AP1" s="22"/>
-      <c r="AQ1" s="22"/>
-      <c r="AR1" s="22"/>
-      <c r="AS1" s="22"/>
-      <c r="AT1" s="22"/>
+      <c r="Q1" s="30"/>
+      <c r="R1" s="30"/>
+      <c r="S1" s="30"/>
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="30"/>
+      <c r="AH1" s="30"/>
+      <c r="AI1" s="30"/>
+      <c r="AJ1" s="30"/>
+      <c r="AK1" s="30"/>
+      <c r="AL1" s="30"/>
+      <c r="AM1" s="30"/>
+      <c r="AN1" s="30"/>
+      <c r="AO1" s="30"/>
+      <c r="AP1" s="30"/>
+      <c r="AQ1" s="30"/>
+      <c r="AR1" s="30"/>
+      <c r="AS1" s="30"/>
+      <c r="AT1" s="30"/>
     </row>
-    <row r="2" spans="1:46" s="18" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="36" t="s">
+    <row r="2" spans="1:46" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="42" t="s">
+      <c r="H2" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="I2" s="42" t="s">
+      <c r="I2" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="J2" s="43" t="s">
+      <c r="J2" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="K2" s="44" t="s">
+      <c r="K2" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="L2" s="44" t="s">
+      <c r="L2" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="M2" s="44" t="s">
+      <c r="M2" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="N2" s="44" t="s">
+      <c r="N2" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="O2" s="45" t="s">
+      <c r="O2" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="P2" s="46" t="s">
+      <c r="P2" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="Q2" s="46" t="s">
+      <c r="Q2" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="R2" s="46" t="s">
+      <c r="R2" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="S2" s="46" t="s">
+      <c r="S2" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="T2" s="46" t="s">
+      <c r="T2" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="U2" s="46" t="s">
+      <c r="U2" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="V2" s="46" t="s">
+      <c r="V2" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="W2" s="46" t="s">
+      <c r="W2" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="X2" s="46" t="s">
+      <c r="X2" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="Y2" s="46" t="s">
+      <c r="Y2" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="Z2" s="46" t="s">
+      <c r="Z2" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="AA2" s="46" t="s">
+      <c r="AA2" s="15" t="s">
         <v>104</v>
       </c>
-      <c r="AB2" s="46" t="s">
+      <c r="AB2" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="AC2" s="46" t="s">
+      <c r="AC2" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="AD2" s="46" t="s">
+      <c r="AD2" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="AE2" s="46" t="s">
+      <c r="AE2" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="AF2" s="46" t="s">
+      <c r="AF2" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="AG2" s="46" t="s">
+      <c r="AG2" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="AH2" s="46" t="s">
+      <c r="AH2" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="AI2" s="46" t="s">
+      <c r="AI2" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="AJ2" s="46" t="s">
+      <c r="AJ2" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="AK2" s="46" t="s">
+      <c r="AK2" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="AL2" s="46" t="s">
+      <c r="AL2" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="AM2" s="46" t="s">
+      <c r="AM2" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="AN2" s="46" t="s">
+      <c r="AN2" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="AO2" s="46" t="s">
+      <c r="AO2" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="AP2" s="46" t="s">
+      <c r="AP2" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="AQ2" s="46" t="s">
+      <c r="AQ2" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="AR2" s="46" t="s">
+      <c r="AR2" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="AS2" s="46" t="s">
+      <c r="AS2" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="AT2" s="46" t="s">
+      <c r="AT2" s="15" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1756,7 +1975,7 @@
       <c r="A3" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="AT3" s="49"/>
+      <c r="AT3"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1774,15 +1993,15 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EFEC405D-8F3B-4A88-81A8-C05C829F992E}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select" xr:uid="{EFEC405D-8F3B-4A88-81A8-C05C829F992E}">
           <x14:formula1>
-            <xm:f>info!$C$2:$C$9</xm:f>
+            <xm:f>options!$C$2:$C$9</xm:f>
           </x14:formula1>
           <xm:sqref>M3</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{78A622A6-5FD1-4C73-8594-7ECF9C674B63}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select" xr:uid="{78A622A6-5FD1-4C73-8594-7ECF9C674B63}">
           <x14:formula1>
-            <xm:f>info!$E$2:$E$3</xm:f>
+            <xm:f>options!$E$2:$E$3</xm:f>
           </x14:formula1>
           <xm:sqref>N3</xm:sqref>
         </x14:dataValidation>
@@ -1794,13 +2013,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2449980B-65A5-4C9A-993B-14CB9F2BDFD7}">
-  <dimension ref="A1:AM3"/>
+  <sheetPr>
+    <tabColor theme="5" tint="0.59999389629810485"/>
+  </sheetPr>
+  <dimension ref="A1:BE3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1809,225 +2031,336 @@
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" customWidth="1"/>
     <col min="5" max="5" width="10.6640625" customWidth="1"/>
-    <col min="10" max="10" width="17.77734375" customWidth="1"/>
-    <col min="11" max="11" width="14" style="7" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1"/>
-    <col min="13" max="13" width="11.33203125" customWidth="1"/>
-    <col min="14" max="14" width="10.6640625" customWidth="1"/>
-    <col min="19" max="19" width="14.109375" customWidth="1"/>
-    <col min="20" max="20" width="16" style="7" customWidth="1"/>
-    <col min="21" max="21" width="12.6640625" customWidth="1"/>
-    <col min="22" max="22" width="11.33203125" customWidth="1"/>
-    <col min="23" max="23" width="10.6640625" customWidth="1"/>
-    <col min="28" max="28" width="14.109375" customWidth="1"/>
-    <col min="29" max="29" width="14" style="7" customWidth="1"/>
-    <col min="30" max="30" width="12.6640625" customWidth="1"/>
-    <col min="31" max="31" width="11.33203125" customWidth="1"/>
-    <col min="32" max="32" width="10.6640625" customWidth="1"/>
-    <col min="37" max="37" width="14.109375" customWidth="1"/>
-    <col min="38" max="38" width="14" style="5" customWidth="1"/>
-    <col min="39" max="39" width="12.44140625" customWidth="1"/>
+    <col min="15" max="17" width="17.77734375" customWidth="1"/>
+    <col min="18" max="18" width="14" style="7" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" customWidth="1"/>
+    <col min="20" max="20" width="11.33203125" customWidth="1"/>
+    <col min="21" max="21" width="10.6640625" customWidth="1"/>
+    <col min="28" max="30" width="14.109375" customWidth="1"/>
+    <col min="31" max="31" width="16" style="7" customWidth="1"/>
+    <col min="32" max="32" width="12.6640625" customWidth="1"/>
+    <col min="33" max="33" width="11.33203125" customWidth="1"/>
+    <col min="34" max="34" width="10.6640625" customWidth="1"/>
+    <col min="41" max="43" width="14.109375" customWidth="1"/>
+    <col min="44" max="44" width="14" style="7" customWidth="1"/>
+    <col min="45" max="45" width="12.6640625" customWidth="1"/>
+    <col min="46" max="46" width="11.33203125" customWidth="1"/>
+    <col min="47" max="47" width="10.6640625" customWidth="1"/>
+    <col min="55" max="56" width="14.109375" customWidth="1"/>
+    <col min="57" max="57" width="14" style="5" customWidth="1"/>
+    <col min="58" max="58" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="B1" s="20" t="s">
+    <row r="1" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="B1" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="19" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="21" t="s">
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27"/>
+      <c r="AF1" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
-      <c r="Y1" s="21"/>
-      <c r="Z1" s="21"/>
-      <c r="AA1" s="21"/>
-      <c r="AB1" s="21"/>
-      <c r="AC1" s="21"/>
-      <c r="AD1" s="25" t="s">
+      <c r="AG1" s="26"/>
+      <c r="AH1" s="26"/>
+      <c r="AI1" s="26"/>
+      <c r="AJ1" s="26"/>
+      <c r="AK1" s="26"/>
+      <c r="AL1" s="26"/>
+      <c r="AM1" s="26"/>
+      <c r="AN1" s="26"/>
+      <c r="AO1" s="26"/>
+      <c r="AP1" s="26"/>
+      <c r="AQ1" s="26"/>
+      <c r="AR1" s="26"/>
+      <c r="AS1" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25"/>
-      <c r="AG1" s="25"/>
-      <c r="AH1" s="25"/>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25"/>
-      <c r="AK1" s="25"/>
-      <c r="AL1" s="26"/>
+      <c r="AT1" s="30"/>
+      <c r="AU1" s="30"/>
+      <c r="AV1" s="30"/>
+      <c r="AW1" s="30"/>
+      <c r="AX1" s="30"/>
+      <c r="AY1" s="30"/>
+      <c r="AZ1" s="30"/>
+      <c r="BA1" s="30"/>
+      <c r="BB1" s="30"/>
+      <c r="BC1" s="30"/>
+      <c r="BD1" s="30"/>
+      <c r="BE1" s="32"/>
     </row>
-    <row r="2" spans="1:39" s="31" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:57" s="16" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="42" t="s">
+        <v>127</v>
+      </c>
+      <c r="J2" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="K2" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="L2" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="M2" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="N2" s="37" t="s">
+        <v>130</v>
+      </c>
+      <c r="O2" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="P2" s="37" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q2" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="28" t="s">
+      <c r="R2" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="S2" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="28" t="s">
+      <c r="T2" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="28" t="s">
+      <c r="U2" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="28" t="s">
+      <c r="V2" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="28" t="s">
+      <c r="W2" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="Q2" s="28" t="s">
+      <c r="X2" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="R2" s="28" t="s">
+      <c r="Y2" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="Z2" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="S2" s="28" t="s">
+      <c r="AA2" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="AB2" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="T2" s="32" t="s">
+      <c r="AC2" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD2" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="AE2" s="40" t="s">
+        <v>143</v>
+      </c>
+      <c r="AF2" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="AG2" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="AH2" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="AI2" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="AJ2" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AK2" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AL2" s="49" t="s">
+        <v>133</v>
+      </c>
+      <c r="AM2" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AN2" s="49" t="s">
+        <v>134</v>
+      </c>
+      <c r="AO2" s="47" t="s">
         <v>30</v>
       </c>
-      <c r="AC2" s="9" t="s">
+      <c r="AP2" s="49" t="s">
+        <v>144</v>
+      </c>
+      <c r="AQ2" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="AD2" s="29" t="s">
+      <c r="AR2" s="50" t="s">
+        <v>145</v>
+      </c>
+      <c r="AS2" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="AE2" s="29" t="s">
+      <c r="AT2" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="AF2" s="29" t="s">
+      <c r="AU2" s="51" t="s">
         <v>34</v>
       </c>
-      <c r="AG2" s="29" t="s">
+      <c r="AV2" s="51" t="s">
         <v>35</v>
       </c>
-      <c r="AH2" s="29" t="s">
+      <c r="AW2" s="51" t="s">
         <v>36</v>
       </c>
-      <c r="AI2" s="29" t="s">
+      <c r="AX2" s="51" t="s">
         <v>49</v>
       </c>
-      <c r="AJ2" s="29" t="s">
+      <c r="AY2" s="52" t="s">
+        <v>135</v>
+      </c>
+      <c r="AZ2" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="AK2" s="29" t="s">
+      <c r="BA2" s="52" t="s">
+        <v>136</v>
+      </c>
+      <c r="BB2" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="AL2" s="29" t="s">
+      <c r="BC2" s="52" t="s">
+        <v>146</v>
+      </c>
+      <c r="BD2" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="AM2" s="30"/>
+      <c r="BE2" s="52" t="s">
+        <v>147</v>
+      </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="AL3" s="49"/>
+    <row r="3" spans="1:57" x14ac:dyDescent="0.3">
+      <c r="R3"/>
+      <c r="AE3"/>
+      <c r="AR3"/>
+      <c r="AY3" s="53"/>
+      <c r="AZ3" s="53"/>
+      <c r="BA3" s="53"/>
+      <c r="BB3" s="53"/>
+      <c r="BC3" s="53"/>
+      <c r="BD3" s="53"/>
+      <c r="BE3" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B1:K1"/>
-    <mergeCell ref="L1:T1"/>
-    <mergeCell ref="U1:AC1"/>
-    <mergeCell ref="AD1:AL1"/>
+    <mergeCell ref="B1:R1"/>
+    <mergeCell ref="S1:AE1"/>
+    <mergeCell ref="AF1:AR1"/>
+    <mergeCell ref="AS1:BE1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="select" xr:uid="{A3F18C05-5A22-4FAE-B7B1-867FB364451F}">
+          <x14:formula1>
+            <xm:f>options!$G$2:$G$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>L1048553 BA3 L3 N3 Y3 AA3 AL3 AN3 AY3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="select" xr:uid="{52B7E54D-8249-4ACA-86FB-99C95F3C1C28}">
+          <x14:formula1>
+            <xm:f>options!$I$2:$I$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>P3 R3 AC3 AE3 AP3 AR3 BC3 BE3</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select" xr:uid="{1AE8C625-C844-47E0-93DE-53765917A448}">
+          <x14:formula1>
+            <xm:f>options!$G$2:$G$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>AY5</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3091F253-E186-473D-8CB7-E5099C6CDCCA}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
+      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.88671875" style="5" customWidth="1"/>
     <col min="2" max="2" width="9.33203125" style="7" customWidth="1"/>
-    <col min="3" max="3" width="16.109375" style="33" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="34" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" style="18" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2037,15 +2370,15 @@
       <c r="B1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="24" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D2" s="48"/>
+      <c r="D2" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2055,9 +2388,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{79FA6A2E-55D0-4BA5-8479-2BFA6A650D99}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select" xr:uid="{79FA6A2E-55D0-4BA5-8479-2BFA6A650D99}">
           <x14:formula1>
-            <xm:f>info!$A$2:$A$5</xm:f>
+            <xm:f>options!$A$2:$A$5</xm:f>
           </x14:formula1>
           <xm:sqref>C2</xm:sqref>
         </x14:dataValidation>
@@ -2069,6 +2402,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.59999389629810485"/>
+  </sheetPr>
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -2093,17 +2429,17 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C1" s="5"/>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="15"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="34"/>
       <c r="H1" s="10"/>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="J1" s="13"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
@@ -2112,7 +2448,7 @@
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -2124,7 +2460,7 @@
       <c r="F2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="12" t="s">
         <v>51</v>
       </c>
       <c r="H2" s="11" t="s">
@@ -2138,7 +2474,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="J3" s="49"/>
+      <c r="J3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2178,10 +2514,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AA73EF4-F459-4FB8-999B-97CF29F368C2}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E3"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2189,9 +2525,11 @@
     <col min="1" max="1" width="23.21875" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
     <col min="5" max="5" width="20.44140625" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>72</v>
       </c>
@@ -2201,8 +2539,14 @@
       <c r="E1" t="s">
         <v>74</v>
       </c>
+      <c r="G1" t="s">
+        <v>137</v>
+      </c>
+      <c r="I1" t="s">
+        <v>150</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>68</v>
       </c>
@@ -2212,8 +2556,14 @@
       <c r="E2" t="s">
         <v>75</v>
       </c>
+      <c r="G2" t="s">
+        <v>139</v>
+      </c>
+      <c r="I2" t="s">
+        <v>149</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -2223,8 +2573,14 @@
       <c r="E3" t="s">
         <v>76</v>
       </c>
+      <c r="G3" t="s">
+        <v>138</v>
+      </c>
+      <c r="I3" t="s">
+        <v>148</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -2232,7 +2588,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -2240,35 +2596,37 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="F10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="3">
+  <tableParts count="5">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>